<commit_message>
added pictures and pdf
</commit_message>
<xml_diff>
--- a/heater-carac.xlsx
+++ b/heater-carac.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Temps (°C)</t>
   </si>
@@ -72,10 +72,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
@@ -712,507 +709,6 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="6.1101211032831421E-2"/>
-          <c:y val="2.0628220113887857E-2"/>
-          <c:w val="0.90485679421651244"/>
-          <c:h val="0.89610258058000003"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Feuil1!$B$31</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Temps (°C)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout/>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Feuil1!$A$32:$A$40</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.125</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.17499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.22500000000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.27500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Feuil1!$B$32:$B$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>48.65</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>67.25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>73.02</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>89.06</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>108.78</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>131.66999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>159.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>195.29</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>231.43</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B2F1-4884-B7D0-6FD2C038F9ED}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1573450751"/>
-        <c:axId val="1573442847"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1573450751"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1573442847"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1573442847"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1573450751"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.7009221184354304"/>
-          <c:y val="0.48148126272467334"/>
-          <c:w val="0.16622841552700648"/>
-          <c:h val="6.3291572877419655E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -1930,46 +1426,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
   <cs:axisTitle>
@@ -2965,536 +2421,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>36739</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>16328</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>8164</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>159203</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3515,20 +2455,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>466726</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>27215</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>122465</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Graphique 4"/>
+        <xdr:cNvPr id="7" name="Graphique 6"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3543,53 +2483,12 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>123826</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>161926</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Graphique 6"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:B12" totalsRowShown="0">
   <autoFilter ref="A1:B12"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Current (mA)" dataDxfId="1"/>
-    <tableColumn id="2" name="Temps (°C)"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A31:B42" totalsRowShown="0">
-  <autoFilter ref="A31:B42"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Current (mA)" dataDxfId="0"/>
     <tableColumn id="2" name="Temps (°C)"/>
@@ -3863,8 +2762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P50" sqref="P50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3972,98 +2871,44 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" t="s">
-        <v>0</v>
-      </c>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="B32">
-        <v>48.65</v>
-      </c>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>0.125</v>
-      </c>
-      <c r="B33">
-        <v>67.25</v>
-      </c>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="B34">
-        <v>73.02</v>
-      </c>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="B35">
-        <v>89.06</v>
-      </c>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="B36">
-        <v>108.78</v>
-      </c>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="B37">
-        <v>131.66999999999999</v>
-      </c>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="B38">
-        <v>159.6</v>
-      </c>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="B39">
-        <v>195.29</v>
-      </c>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="B40">
-        <v>231.43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="1">
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "added pictures and pdf"
This reverts commit 612e7ac8cb960e428ae3828db318b95c8038de49.
</commit_message>
<xml_diff>
--- a/heater-carac.xlsx
+++ b/heater-carac.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Temps (°C)</t>
   </si>
@@ -72,7 +72,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
@@ -709,6 +712,507 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.1101211032831421E-2"/>
+          <c:y val="2.0628220113887857E-2"/>
+          <c:w val="0.90485679421651244"/>
+          <c:h val="0.89610258058000003"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$B$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Temps (°C)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$A$32:$A$40</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.22500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.27500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$B$32:$B$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>48.65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>108.78</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>131.66999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>159.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>195.29</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>231.43</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B2F1-4884-B7D0-6FD2C038F9ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1573450751"/>
+        <c:axId val="1573442847"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1573450751"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1573442847"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1573442847"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1573450751"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.7009221184354304"/>
+          <c:y val="0.48148126272467334"/>
+          <c:w val="0.16622841552700648"/>
+          <c:h val="6.3291572877419655E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -1426,6 +1930,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
   <cs:axisTitle>
@@ -2421,20 +2965,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>36739</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>16328</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>8164</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>159203</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2455,20 +3515,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27214</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>27215</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>466726</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>27214</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>122465</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Graphique 6"/>
+        <xdr:cNvPr id="5" name="Graphique 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2483,12 +3543,53 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Graphique 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:B12" totalsRowShown="0">
   <autoFilter ref="A1:B12"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Current (mA)" dataDxfId="1"/>
+    <tableColumn id="2" name="Temps (°C)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A31:B42" totalsRowShown="0">
+  <autoFilter ref="A31:B42"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Current (mA)" dataDxfId="0"/>
     <tableColumn id="2" name="Temps (°C)"/>
@@ -2762,8 +3863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P50" sqref="P50"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2871,44 +3972,98 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="B32">
+        <v>48.65</v>
+      </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="B33">
+        <v>67.25</v>
+      </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="B34">
+        <v>73.02</v>
+      </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="B35">
+        <v>89.06</v>
+      </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="B36">
+        <v>108.78</v>
+      </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="B37">
+        <v>131.66999999999999</v>
+      </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="B38">
+        <v>159.6</v>
+      </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="B39">
+        <v>195.29</v>
+      </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="B40">
+        <v>231.43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>